<commit_message>
chore: add output to gitignore and update account config
</commit_message>
<xml_diff>
--- a/datas/__beans__.xlsx
+++ b/datas/__beans__.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="30240" windowHeight="13620" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="144525" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="21">
     <font>
       <name val="等线"/>
       <charset val="134"/>
@@ -26,14 +26,14 @@
     </font>
     <font>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="134"/>
       <color rgb="FF9C0006"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="134"/>
       <color rgb="FF006100"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -41,20 +41,142 @@
     <font>
       <name val="等线"/>
       <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="等线"/>
       <charset val="134"/>
-      <family val="3"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="0"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
@@ -73,8 +195,182 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -82,15 +378,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -98,21 +630,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="22">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -438,7 +1016,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -448,22 +1025,34 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col width="20.625" customWidth="1" style="4" min="2" max="2"/>
-    <col width="29.875" customWidth="1" style="4" min="3" max="5"/>
-    <col width="15" customWidth="1" style="4" min="6" max="9"/>
-    <col width="13.5" customWidth="1" style="4" min="10" max="13"/>
+    <col width="6.35714285714286" customWidth="1" style="1" min="1" max="1"/>
+    <col width="22.1428571428571" customWidth="1" style="1" min="2" max="2"/>
+    <col width="78" customWidth="1" style="1" min="3" max="3"/>
+    <col width="11.7142857142857" customWidth="1" style="1" min="4" max="4"/>
+    <col width="5.57142857142857" customWidth="1" style="1" min="5" max="5"/>
+    <col width="7.57142857142857" customWidth="1" style="1" min="6" max="6"/>
+    <col width="14" customWidth="1" style="1" min="7" max="7"/>
+    <col width="4.71428571428571" customWidth="1" style="1" min="8" max="8"/>
+    <col width="5.78571428571429" customWidth="1" style="1" min="9" max="9"/>
+    <col width="23.2857142857143" customWidth="1" style="1" min="10" max="10"/>
+    <col width="5.57142857142857" customWidth="1" style="1" min="11" max="11"/>
+    <col width="17.0714285714286" customWidth="1" style="1" min="12" max="12"/>
+    <col width="5.78571428571429" customWidth="1" style="1" min="13" max="13"/>
+    <col width="25.1428571428571" customWidth="1" style="1" min="14" max="14"/>
+    <col width="4.71428571428571" customWidth="1" style="1" min="15" max="15"/>
+    <col width="7.64285714285714" customWidth="1" style="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>##var</t>
         </is>
@@ -515,7 +1104,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>##var</t>
         </is>
@@ -525,7 +1114,7 @@
           <t>name</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="K2" s="4" t="inlineStr">
         <is>
           <t>alias</t>
         </is>
@@ -550,7 +1139,7 @@
           <t>tags</t>
         </is>
       </c>
-      <c r="P2" s="2" t="inlineStr">
+      <c r="P2" s="4" t="inlineStr">
         <is>
           <t>variants</t>
         </is>
@@ -592,7 +1181,7 @@
           <t>字段名</t>
         </is>
       </c>
-      <c r="K3" s="2" t="inlineStr">
+      <c r="K3" s="4" t="inlineStr">
         <is>
           <t>别名</t>
         </is>
@@ -1260,68 +1849,51 @@
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="0" t="inlineStr">
+      <c r="J32" s="0" t="n"/>
+      <c r="L32" s="0" t="n"/>
+      <c r="M32" s="0" t="n"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>ShopItemBase</t>
         </is>
       </c>
-      <c r="G32" s="0" t="inlineStr">
+      <c r="G33" s="0" t="inlineStr">
         <is>
           <t>商店道具基类</t>
         </is>
       </c>
-      <c r="I32" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="J32" s="0" t="inlineStr">
+      <c r="I33" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="J33" s="0" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="L32" s="0" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="M32" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="N32" s="0" t="inlineStr">
+      <c r="L33" s="0" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="M33" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N33" s="0" t="inlineStr">
         <is>
           <t>配置ID</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="J33" s="0" t="inlineStr">
-        <is>
-          <t>shop_id</t>
-        </is>
-      </c>
-      <c r="L33" s="0" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="M33" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="N33" s="0" t="inlineStr">
-        <is>
-          <t>所属商店ID</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="J34" s="0" t="inlineStr">
         <is>
-          <t>item_id</t>
+          <t>shop_id</t>
         </is>
       </c>
       <c r="L34" s="0" t="inlineStr">
@@ -1336,19 +1908,19 @@
       </c>
       <c r="N34" s="0" t="inlineStr">
         <is>
-          <t>道具ID</t>
+          <t>所属商店ID</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="J35" s="0" t="inlineStr">
         <is>
-          <t>currency_type</t>
+          <t>item_id</t>
         </is>
       </c>
       <c r="L35" s="0" t="inlineStr">
         <is>
-          <t>CurrencyType</t>
+          <t>int</t>
         </is>
       </c>
       <c r="M35" s="0" t="inlineStr">
@@ -1358,19 +1930,19 @@
       </c>
       <c r="N35" s="0" t="inlineStr">
         <is>
-          <t>货币类型</t>
+          <t>道具ID</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="J36" s="0" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>currency_type</t>
         </is>
       </c>
       <c r="L36" s="0" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>CurrencyType</t>
         </is>
       </c>
       <c r="M36" s="0" t="inlineStr">
@@ -1380,14 +1952,14 @@
       </c>
       <c r="N36" s="0" t="inlineStr">
         <is>
-          <t>价格</t>
+          <t>货币类型</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="J37" s="0" t="inlineStr">
         <is>
-          <t>discount</t>
+          <t>price</t>
         </is>
       </c>
       <c r="L37" s="0" t="inlineStr">
@@ -1402,19 +1974,19 @@
       </c>
       <c r="N37" s="0" t="inlineStr">
         <is>
-          <t>折扣百分比</t>
+          <t>价格</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="J38" s="0" t="inlineStr">
         <is>
-          <t>stock_type</t>
+          <t>discount</t>
         </is>
       </c>
       <c r="L38" s="0" t="inlineStr">
         <is>
-          <t>StockType</t>
+          <t>int</t>
         </is>
       </c>
       <c r="M38" s="0" t="inlineStr">
@@ -1424,19 +1996,19 @@
       </c>
       <c r="N38" s="0" t="inlineStr">
         <is>
-          <t>库存类型</t>
+          <t>折扣百分比</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="J39" s="0" t="inlineStr">
         <is>
-          <t>stock_limit</t>
+          <t>stock_type</t>
         </is>
       </c>
       <c r="L39" s="0" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>StockType</t>
         </is>
       </c>
       <c r="M39" s="0" t="inlineStr">
@@ -1446,14 +2018,14 @@
       </c>
       <c r="N39" s="0" t="inlineStr">
         <is>
-          <t>库存数量</t>
+          <t>库存类型</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="J40" s="0" t="inlineStr">
         <is>
-          <t>unlock_level</t>
+          <t>stock_limit</t>
         </is>
       </c>
       <c r="L40" s="0" t="inlineStr">
@@ -1468,14 +2040,14 @@
       </c>
       <c r="N40" s="0" t="inlineStr">
         <is>
-          <t>解锁等级</t>
+          <t>库存数量</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="J41" s="0" t="inlineStr">
         <is>
-          <t>position</t>
+          <t>unlock_level</t>
         </is>
       </c>
       <c r="L41" s="0" t="inlineStr">
@@ -1485,24 +2057,24 @@
       </c>
       <c r="M41" s="0" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>c;s</t>
         </is>
       </c>
       <c r="N41" s="0" t="inlineStr">
         <is>
-          <t>显示位置</t>
+          <t>解锁等级</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="J42" s="0" t="inlineStr">
         <is>
-          <t>is_hot</t>
+          <t>position</t>
         </is>
       </c>
       <c r="L42" s="0" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>int</t>
         </is>
       </c>
       <c r="M42" s="0" t="inlineStr">
@@ -1512,14 +2084,14 @@
       </c>
       <c r="N42" s="0" t="inlineStr">
         <is>
-          <t>热卖标签</t>
+          <t>显示位置</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="J43" s="0" t="inlineStr">
         <is>
-          <t>is_new</t>
+          <t>is_hot</t>
         </is>
       </c>
       <c r="L43" s="0" t="inlineStr">
@@ -1534,100 +2106,63 @@
       </c>
       <c r="N43" s="0" t="inlineStr">
         <is>
-          <t>新品标签</t>
+          <t>热卖标签</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="J44" s="0" t="inlineStr">
         <is>
+          <t>is_new</t>
+        </is>
+      </c>
+      <c r="L44" s="0" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="M44" s="0" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="N44" s="0" t="inlineStr">
+        <is>
+          <t>新品标签</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="J45" s="0" t="inlineStr">
+        <is>
           <t>is_recommend</t>
         </is>
       </c>
-      <c r="L44" s="0" t="inlineStr">
+      <c r="L45" s="0" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="M44" s="0" t="inlineStr">
+      <c r="M45" s="0" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="N44" s="0" t="inlineStr">
+      <c r="N45" s="0" t="inlineStr">
         <is>
           <t>推荐标签</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="B45" s="0" t="inlineStr">
-        <is>
-          <t>ShopItemNormal</t>
-        </is>
-      </c>
-      <c r="C45" s="0" t="inlineStr">
-        <is>
-          <t>ShopItemBase</t>
-        </is>
-      </c>
-      <c r="G45" s="0" t="inlineStr">
-        <is>
-          <t>普通商店道具</t>
-        </is>
-      </c>
-      <c r="I45" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-    </row>
     <row r="46">
-      <c r="B46" s="0" t="inlineStr">
-        <is>
-          <t>ShopItemMystery</t>
-        </is>
-      </c>
-      <c r="C46" s="0" t="inlineStr">
-        <is>
-          <t>ShopItemBase</t>
-        </is>
-      </c>
-      <c r="G46" s="0" t="inlineStr">
-        <is>
-          <t>神秘商店道具</t>
-        </is>
-      </c>
-      <c r="I46" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="J46" s="0" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="L46" s="0" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="M46" s="0" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="N46" s="0" t="inlineStr">
-        <is>
-          <t>权重（0=固定出现）</t>
-        </is>
-      </c>
+      <c r="J46" s="0" t="n"/>
+      <c r="L46" s="0" t="n"/>
+      <c r="M46" s="0" t="n"/>
     </row>
     <row r="47">
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>ShopItemGuild</t>
+          <t>ShopItemNormal</t>
         </is>
       </c>
       <c r="C47" s="0" t="inlineStr">
@@ -1637,7 +2172,7 @@
       </c>
       <c r="G47" s="0" t="inlineStr">
         <is>
-          <t>公会商店道具</t>
+          <t>普通商店道具</t>
         </is>
       </c>
       <c r="I47" s="0" t="inlineStr">
@@ -1645,53 +2180,17 @@
           <t>c;s</t>
         </is>
       </c>
-      <c r="J47" s="0" t="inlineStr">
-        <is>
-          <t>guild_level_require</t>
-        </is>
-      </c>
-      <c r="L47" s="0" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="M47" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="N47" s="0" t="inlineStr">
-        <is>
-          <t>公会等级要求</t>
-        </is>
-      </c>
     </row>
     <row r="48">
-      <c r="J48" s="0" t="inlineStr">
-        <is>
-          <t>guild_contribution_min</t>
-        </is>
-      </c>
-      <c r="L48" s="0" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="M48" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="N48" s="0" t="inlineStr">
-        <is>
-          <t>公会贡献度要求</t>
-        </is>
-      </c>
+      <c r="B48" s="0" t="n"/>
+      <c r="C48" s="0" t="n"/>
+      <c r="G48" s="0" t="n"/>
+      <c r="I48" s="0" t="n"/>
     </row>
     <row r="49">
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>ShopItemAlliance</t>
+          <t>ShopItemMystery</t>
         </is>
       </c>
       <c r="C49" s="0" t="inlineStr">
@@ -1701,7 +2200,7 @@
       </c>
       <c r="G49" s="0" t="inlineStr">
         <is>
-          <t>联盟商店道具</t>
+          <t>神秘商店道具</t>
         </is>
       </c>
       <c r="I49" s="0" t="inlineStr">
@@ -1711,7 +2210,7 @@
       </c>
       <c r="J49" s="0" t="inlineStr">
         <is>
-          <t>alliance_level_require</t>
+          <t>weight</t>
         </is>
       </c>
       <c r="L49" s="0" t="inlineStr">
@@ -1721,41 +2220,28 @@
       </c>
       <c r="M49" s="0" t="inlineStr">
         <is>
-          <t>c;s</t>
+          <t>s</t>
         </is>
       </c>
       <c r="N49" s="0" t="inlineStr">
         <is>
-          <t>联盟等级要求</t>
+          <t>权重（0=固定出现）</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="J50" s="0" t="inlineStr">
-        <is>
-          <t>alliance_contribution_min</t>
-        </is>
-      </c>
-      <c r="L50" s="0" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="M50" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="N50" s="0" t="inlineStr">
-        <is>
-          <t>联盟贡献度要求</t>
-        </is>
-      </c>
+      <c r="B50" s="0" t="n"/>
+      <c r="C50" s="0" t="n"/>
+      <c r="G50" s="0" t="n"/>
+      <c r="I50" s="0" t="n"/>
+      <c r="J50" s="0" t="n"/>
+      <c r="L50" s="0" t="n"/>
+      <c r="M50" s="0" t="n"/>
     </row>
     <row r="51">
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>ShopItemTimeLimited</t>
+          <t>ShopItemGuild</t>
         </is>
       </c>
       <c r="C51" s="0" t="inlineStr">
@@ -1765,7 +2251,7 @@
       </c>
       <c r="G51" s="0" t="inlineStr">
         <is>
-          <t>限时商店道具</t>
+          <t>公会商店道具</t>
         </is>
       </c>
       <c r="I51" s="0" t="inlineStr">
@@ -1775,12 +2261,12 @@
       </c>
       <c r="J51" s="0" t="inlineStr">
         <is>
-          <t>start_time</t>
+          <t>guild_level_require</t>
         </is>
       </c>
       <c r="L51" s="0" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>int</t>
         </is>
       </c>
       <c r="M51" s="0" t="inlineStr">
@@ -1790,29 +2276,253 @@
       </c>
       <c r="N51" s="0" t="inlineStr">
         <is>
-          <t>开始时间（Unix时间戳）</t>
+          <t>公会等级要求</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="J52" s="0" t="inlineStr">
         <is>
+          <t>guild_contribution_min</t>
+        </is>
+      </c>
+      <c r="L52" s="0" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="M52" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N52" s="0" t="inlineStr">
+        <is>
+          <t>公会贡献度要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="J53" s="0" t="n"/>
+      <c r="L53" s="0" t="n"/>
+      <c r="M53" s="0" t="n"/>
+    </row>
+    <row r="54">
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>ShopItemAlliance</t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="inlineStr">
+        <is>
+          <t>ShopItemBase</t>
+        </is>
+      </c>
+      <c r="G54" s="0" t="inlineStr">
+        <is>
+          <t>联盟商店道具</t>
+        </is>
+      </c>
+      <c r="I54" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="J54" s="0" t="inlineStr">
+        <is>
+          <t>alliance_level_require</t>
+        </is>
+      </c>
+      <c r="L54" s="0" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="M54" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N54" s="0" t="inlineStr">
+        <is>
+          <t>联盟等级要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="J55" s="0" t="inlineStr">
+        <is>
+          <t>alliance_contribution_min</t>
+        </is>
+      </c>
+      <c r="L55" s="0" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="M55" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N55" s="0" t="inlineStr">
+        <is>
+          <t>联盟贡献度要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="J56" s="0" t="n"/>
+      <c r="L56" s="0" t="n"/>
+      <c r="M56" s="0" t="n"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>ShopItemTimeLimited</t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="inlineStr">
+        <is>
+          <t>ShopItemBase</t>
+        </is>
+      </c>
+      <c r="G57" s="0" t="inlineStr">
+        <is>
+          <t>限时商店道具</t>
+        </is>
+      </c>
+      <c r="I57" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="J57" s="0" t="inlineStr">
+        <is>
+          <t>start_time</t>
+        </is>
+      </c>
+      <c r="L57" s="0" t="inlineStr">
+        <is>
+          <t>datetime</t>
+        </is>
+      </c>
+      <c r="M57" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N57" s="0" t="inlineStr">
+        <is>
+          <t>开始时间（Unix时间戳）</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="J58" s="0" t="inlineStr">
+        <is>
           <t>end_time</t>
         </is>
       </c>
-      <c r="L52" s="0" t="inlineStr">
+      <c r="L58" s="0" t="inlineStr">
         <is>
           <t>datetime</t>
         </is>
       </c>
-      <c r="M52" s="0" t="inlineStr">
-        <is>
-          <t>c;s</t>
-        </is>
-      </c>
-      <c r="N52" s="0" t="inlineStr">
+      <c r="M58" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N58" s="0" t="inlineStr">
         <is>
           <t>结束时间（Unix时间戳）</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="J59" s="0" t="n"/>
+      <c r="L59" s="0" t="n"/>
+      <c r="M59" s="0" t="n"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="G60" s="0" t="inlineStr">
+        <is>
+          <t>账号</t>
+        </is>
+      </c>
+      <c r="I60" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="J60" s="0" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L60" s="0" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="M60" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N60" s="0" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="J61" s="0" t="inlineStr">
+        <is>
+          <t>user_name</t>
+        </is>
+      </c>
+      <c r="L61" s="0" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="M61" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N61" s="0" t="inlineStr">
+        <is>
+          <t>账号</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="J62" s="0" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+      <c r="L62" s="0" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="M62" s="0" t="inlineStr">
+        <is>
+          <t>c;s</t>
+        </is>
+      </c>
+      <c r="N62" s="0" t="inlineStr">
+        <is>
+          <t>密码</t>
         </is>
       </c>
     </row>

</xml_diff>